<commit_message>
Add print/White and Black
</commit_message>
<xml_diff>
--- a/out/aaa.xlsx
+++ b/out/aaa.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\gitwork\CreateTableOfContentsExcelUsingSheetNames\out\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E238C330-B05C-438C-8C48-B43F62654437}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{79541AD1-16F5-4B3A-8E9B-69DED4F31174}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1060" yWindow="1060" windowWidth="19040" windowHeight="12700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2280" yWindow="2280" windowWidth="19040" windowHeight="12700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="２ページ" sheetId="4" r:id="rId1"/>

</xml_diff>